<commit_message>
Lyso PL identification functional
NewFeatures:
+ Add: Identify Lyso PLs

BugFix:
+ Fixed: Lyso PL prediction
+ Fixed: Lyso PL / DG image generation
</commit_message>
<xml_diff>
--- a/ConfigurationFiles/1-FA_Whitelist_LPL.xlsx
+++ b/ConfigurationFiles/1-FA_Whitelist_LPL.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5424E9-4E8E-4633-9E99-05078DF39210}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="8475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="8480"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -232,7 +231,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -543,19 +542,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E56"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56:E62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -578,7 +577,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -601,7 +600,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>63</v>
       </c>
@@ -624,7 +623,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -647,7 +646,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>65</v>
       </c>
@@ -670,7 +669,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -693,7 +692,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>66</v>
       </c>
@@ -716,7 +715,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -739,7 +738,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>61</v>
       </c>
@@ -762,7 +761,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -785,7 +784,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -808,7 +807,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -831,7 +830,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -854,7 +853,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -877,7 +876,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -900,7 +899,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -923,7 +922,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -946,7 +945,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -969,7 +968,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -992,7 +991,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -1015,7 +1014,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -1038,7 +1037,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -1061,7 +1060,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -1084,7 +1083,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -1107,7 +1106,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -1130,7 +1129,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>52</v>
       </c>
@@ -1153,7 +1152,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -1176,7 +1175,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -1199,7 +1198,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -1222,7 +1221,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -1245,7 +1244,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1268,7 +1267,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>46</v>
       </c>
@@ -1291,7 +1290,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>47</v>
       </c>
@@ -1314,7 +1313,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -1337,7 +1336,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>23</v>
       </c>
@@ -1360,7 +1359,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>30</v>
       </c>
@@ -1383,7 +1382,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>31</v>
       </c>
@@ -1406,7 +1405,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -1429,7 +1428,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -1452,7 +1451,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -1475,7 +1474,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>24</v>
       </c>
@@ -1498,7 +1497,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>32</v>
       </c>
@@ -1521,7 +1520,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>33</v>
       </c>
@@ -1544,7 +1543,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>34</v>
       </c>
@@ -1567,7 +1566,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>9</v>
       </c>
@@ -1590,7 +1589,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>10</v>
       </c>
@@ -1613,7 +1612,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>11</v>
       </c>
@@ -1633,7 +1632,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>50</v>
       </c>
@@ -1653,7 +1652,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>25</v>
       </c>
@@ -1673,7 +1672,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>35</v>
       </c>
@@ -1693,7 +1692,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>36</v>
       </c>
@@ -1713,7 +1712,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>37</v>
       </c>
@@ -1733,7 +1732,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>67</v>
       </c>
@@ -1753,7 +1752,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>26</v>
       </c>
@@ -1773,7 +1772,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>38</v>
       </c>
@@ -1793,7 +1792,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>39</v>
       </c>
@@ -1813,7 +1812,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>12</v>
       </c>
@@ -1827,7 +1826,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>13</v>
       </c>
@@ -1841,7 +1840,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>14</v>
       </c>
@@ -1855,7 +1854,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>15</v>
       </c>
@@ -1869,7 +1868,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>16</v>
       </c>
@@ -1883,7 +1882,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>17</v>
       </c>

</xml_diff>